<commit_message>
added responsive skeleton to all content
</commit_message>
<xml_diff>
--- a/misc/tasklist.xlsx
+++ b/misc/tasklist.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlang\Documents\Web Development\mlang251.github.io\misc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="13395" windowHeight="7740"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="13398" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Completed</t>
   </si>
@@ -40,12 +45,15 @@
   </si>
   <si>
     <t>Content</t>
+  </si>
+  <si>
+    <t>Turn section#about other interests ul into an inline-block list with thumbnail pic next to each li that compliments the li</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -124,6 +132,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -171,7 +182,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -204,9 +215,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -239,6 +267,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -415,21 +460,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.83984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="89" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -440,28 +485,33 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -477,7 +527,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -489,7 +539,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
made responsive landing navigation
</commit_message>
<xml_diff>
--- a/misc/tasklist.xlsx
+++ b/misc/tasklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Event</t>
   </si>
@@ -48,28 +48,16 @@
     <t>Document code</t>
   </si>
   <si>
-    <t>When nav item is clicked</t>
-  </si>
-  <si>
-    <t>Smooth scroll to section</t>
-  </si>
-  <si>
     <t>When header is scrolled above section#about</t>
   </si>
   <si>
     <t>Re-attach nav menu in section#landing</t>
   </si>
   <si>
-    <t>When viewport is medium</t>
-  </si>
-  <si>
-    <t>Stack nav items in 2 rows of 2</t>
-  </si>
-  <si>
-    <t>When viewport is small</t>
-  </si>
-  <si>
-    <t>Turn nav items into dropdown menu</t>
+    <t>Touch screen anchor click</t>
+  </si>
+  <si>
+    <t>Change font color back after click</t>
   </si>
 </sst>
 </file>
@@ -448,11 +436,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,42 +499,22 @@
     </row>
     <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made text wrap image
</commit_message>
<xml_diff>
--- a/misc/tasklist.xlsx
+++ b/misc/tasklist.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlang\Documents\Web Development\mlang251.github.io\misc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="13395" windowHeight="7740"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="13398" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Event</t>
   </si>
@@ -37,9 +42,6 @@
   </si>
   <si>
     <t>Attach resume</t>
-  </si>
-  <si>
-    <t>Headshot in header to the left of name and email</t>
   </si>
   <si>
     <t>Update Linkedin</t>
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -192,7 +194,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -225,9 +227,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -260,6 +279,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -436,20 +472,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="108.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="108.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -457,64 +493,59 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="11" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -529,7 +560,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -541,7 +572,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
made responsive table for skills section
</commit_message>
<xml_diff>
--- a/misc/tasklist.xlsx
+++ b/misc/tasklist.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Completed</t>
   </si>
@@ -30,9 +30,6 @@
   </si>
   <si>
     <t>Task</t>
-  </si>
-  <si>
-    <t>Combine section#goals unordered lists into a single responsive table</t>
   </si>
   <si>
     <t>When header is scrolled below section#landing</t>
@@ -460,11 +457,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -487,32 +484,27 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="C7" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>